<commit_message>
format updates / tidy
</commit_message>
<xml_diff>
--- a/WxSatInfo.xlsx
+++ b/WxSatInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crein\OneDrive\Documents\GitHub\wxcapture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Users\mike\Documents\GitHub\wxcapture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92B7210-87FE-451A-BF6F-7A590F4B2C95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31CC0B4-0867-44AB-9D70-2B052B1B9511}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14745" yWindow="675" windowWidth="33510" windowHeight="19215" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GOES 16 &amp; 17" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Electro-L N2" sheetId="4" r:id="rId5"/>
     <sheet name="EWS-G1" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -315,15 +315,6 @@
     <t>Product Name</t>
   </si>
   <si>
-    <t>GOES-16</t>
-  </si>
-  <si>
-    <t>Availability</t>
-  </si>
-  <si>
-    <t>GOES-17</t>
-  </si>
-  <si>
     <t>Period-Min(s)</t>
   </si>
   <si>
@@ -467,6 +458,17 @@
     <t xml:space="preserve"> Manually
 entered in response
 to events</t>
+  </si>
+  <si>
+    <t>GOES 16 and 17 - Detail</t>
+  </si>
+  <si>
+    <t>GOES-16
+Availability</t>
+  </si>
+  <si>
+    <t>GOES-17
+Availability</t>
   </si>
 </sst>
 </file>
@@ -556,22 +558,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -581,37 +574,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -998,9 +1001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:H11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1012,27 +1013,27 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1043,18 +1044,18 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -1063,21 +1064,21 @@
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="13" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -1086,19 +1087,19 @@
       <c r="B11" s="4">
         <v>0.47</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -1107,19 +1108,19 @@
       <c r="B12" s="4">
         <v>0.64</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
     </row>
     <row r="13" spans="1:13" ht="23.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -1128,19 +1129,19 @@
       <c r="B13" s="4">
         <v>0.86</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
@@ -1149,19 +1150,19 @@
       <c r="B14" s="4">
         <v>1.37</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -1170,19 +1171,19 @@
       <c r="B15" s="4">
         <v>1.6</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
@@ -1191,19 +1192,19 @@
       <c r="B16" s="4">
         <v>2.2400000000000002</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
@@ -1212,19 +1213,19 @@
       <c r="B17" s="4">
         <v>3.9</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
@@ -1233,19 +1234,19 @@
       <c r="B18" s="4">
         <v>6.2</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
@@ -1254,19 +1255,19 @@
       <c r="B19" s="4">
         <v>6.9</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
@@ -1275,19 +1276,19 @@
       <c r="B20" s="4">
         <v>7.3</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
     </row>
     <row r="21" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -1296,19 +1297,19 @@
       <c r="B21" s="4">
         <v>8.4</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -1317,19 +1318,19 @@
       <c r="B22" s="4">
         <v>9.6</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
     </row>
     <row r="23" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
@@ -1338,21 +1339,21 @@
       <c r="B23" s="4">
         <v>10.3</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="7" t="s">
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
     </row>
     <row r="24" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
@@ -1361,19 +1362,19 @@
       <c r="B24" s="4">
         <v>11.2</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
@@ -1382,19 +1383,19 @@
       <c r="B25" s="4">
         <v>12.3</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
     </row>
     <row r="26" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
@@ -1403,52 +1404,22 @@
       <c r="B26" s="4">
         <v>13.3</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="I12:M12"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="I13:M13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="I14:M14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="I15:M15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="I16:M16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="I18:M18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="I19:M19"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="I20:M20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="I21:M21"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="I22:M22"/>
     <mergeCell ref="C26:H26"/>
     <mergeCell ref="I26:M26"/>
     <mergeCell ref="C23:H23"/>
@@ -1457,6 +1428,36 @@
     <mergeCell ref="I24:M24"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="I25:M25"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="I21:M21"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="I22:M22"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="I14:M14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="I15:M15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="I16:M16"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="I13:M13"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="I10:M10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -1468,510 +1469,521 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E886E89E-DF11-4970-BDF2-1AAFA142AD93}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
     <col min="8" max="8" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:8" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C4" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="F4" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" s="20" t="s">
+      <c r="C5" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="16">
+        <v>60</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="20"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="G5" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="H5" s="20"/>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>1</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E3" s="16">
-        <v>60</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="C6" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="18">
+        <v>15</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G6" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="H6" s="20"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
-        <v>1</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="E4" s="25">
-        <v>15</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5" s="16">
-        <v>30</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E6" s="16">
-        <v>30</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>109</v>
-      </c>
       <c r="C7" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E7" s="16">
         <v>30</v>
       </c>
       <c r="F7" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="H7" s="20"/>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>110</v>
-      </c>
       <c r="C8" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E8" s="16">
         <v>30</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>107</v>
+        <v>104</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>111</v>
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E9" s="16">
         <v>30</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G9" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" s="20"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>112</v>
-      </c>
       <c r="C10" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E10" s="16">
         <v>30</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>107</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>113</v>
+      <c r="A11" s="4">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E11" s="16">
         <v>30</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>107</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12" s="16"/>
+      <c r="A12" s="4">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>98</v>
+      </c>
       <c r="D12" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E12" s="16">
         <v>30</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>134</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="H12" s="20"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>115</v>
+      <c r="A13" s="4">
+        <v>15</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" s="16"/>
+        <v>98</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>98</v>
+      </c>
       <c r="E13" s="16">
         <v>30</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>107</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="4">
+        <v>16</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="16">
+        <v>30</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>17</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16">
+        <v>30</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>21</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E14" s="16" t="s">
+      <c r="C17" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>22</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="C18" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="G14" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="G18" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="19" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>24</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="16">
+        <v>60</v>
+      </c>
+      <c r="F19" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="F15" s="16" t="s">
+      <c r="G19" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>25</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>30</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G15" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="H15" s="16" t="s">
+      <c r="C21" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21" s="19" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
-        <v>24</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E17" s="16">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>32</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="H22" s="20"/>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>60</v>
       </c>
-      <c r="F17" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
-        <v>25</v>
-      </c>
-      <c r="B18" s="22" t="s">
+      <c r="B23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="16">
+        <v>60</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="H23" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s">
-        <v>125</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>133</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>60</v>
-      </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E21" s="16">
-        <v>60</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>135</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2028,76 +2040,76 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="7" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="4"/>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="6" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="4"/>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="6" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2122,9 +2134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2170,13 +2180,13 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -2185,19 +2195,19 @@
       <c r="B10" s="4">
         <v>10.4</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2215,9 +2225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2261,13 +2269,13 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -2276,21 +2284,21 @@
       <c r="B10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="7" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -2299,21 +2307,21 @@
       <c r="B11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="7" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -2322,21 +2330,21 @@
       <c r="B12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="7" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -2345,21 +2353,21 @@
       <c r="B13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7" t="s">
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -2368,21 +2376,21 @@
       <c r="B14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="7" t="s">
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -2391,21 +2399,21 @@
       <c r="B15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="7" t="s">
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -2414,21 +2422,21 @@
       <c r="B16" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="7" t="s">
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -2437,21 +2445,21 @@
       <c r="B17" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="7" t="s">
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -2460,21 +2468,21 @@
       <c r="B18" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="7" t="s">
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -2483,80 +2491,62 @@
       <c r="B19" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="7" t="s">
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>10</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="7" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
     </row>
     <row r="21" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="6" t="s">
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="I12:M12"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="I13:M13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="I14:M14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="I15:M15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="I16:M16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="I17:M17"/>
     <mergeCell ref="C21:H21"/>
     <mergeCell ref="I21:M21"/>
     <mergeCell ref="C18:H18"/>
@@ -2565,6 +2555,24 @@
     <mergeCell ref="I19:M19"/>
     <mergeCell ref="C20:H20"/>
     <mergeCell ref="I20:M20"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="I15:M15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="I16:M16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="I13:M13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="I14:M14"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="I11:M11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
@@ -2578,9 +2586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2626,13 +2632,13 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -2641,19 +2647,19 @@
       <c r="B10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -2662,19 +2668,19 @@
       <c r="B11" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -2683,19 +2689,19 @@
       <c r="B12" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -2704,19 +2710,19 @@
       <c r="B13" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
@@ -2725,34 +2731,34 @@
       <c r="B14" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="I13:M13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="I14:M14"/>
     <mergeCell ref="C9:H9"/>
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="C10:H10"/>
     <mergeCell ref="I10:M10"/>
     <mergeCell ref="C11:H11"/>
     <mergeCell ref="I11:M11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="I12:M12"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="I13:M13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="I14:M14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>

</xml_diff>